<commit_message>
Updated timesheet, setup to merge into main
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C5AB7B-EAB8-40CB-94DE-150AE1577899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033F8475-2CF7-4C71-A242-366EC97F3547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -113,7 +113,7 @@
     <t>Frontend Dev</t>
   </si>
   <si>
-    <t>Reimplemented persistent bottom nav bar, updated documentation in repo</t>
+    <t>Reimplemented persistent bottom nav bar, fixed merge conflicts, cleaning up fStack branch</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <dimension ref="A1:G199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,7 +707,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>0.83055555555555582</v>
+        <v>0.84722222222222243</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -913,11 +913,11 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="D12" s="9">
-        <v>0.61250000000000004</v>
+        <v>0.62916666666666665</v>
       </c>
       <c r="E12" s="10">
         <f t="shared" si="0"/>
-        <v>3.9583333333333415E-2</v>
+        <v>5.6250000000000022E-2</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Updated sab timesheet with changes made to the frontend code
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033F8475-2CF7-4C71-A242-366EC97F3547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80003F6-FF98-4C6C-B416-CEDC0CC28B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Name:</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Research</t>
   </si>
   <si>
-    <t>Check-in: Group meetign with Tyler, discussed what was needed for the pre-alpha build, planning more research for app development</t>
-  </si>
-  <si>
     <t>Researching how to implement and use Flutter in conjunction with MongoDB, watching tutorials on how to use Dart</t>
   </si>
   <si>
@@ -114,6 +111,18 @@
   </si>
   <si>
     <t>Reimplemented persistent bottom nav bar, fixed merge conflicts, cleaning up fStack branch</t>
+  </si>
+  <si>
+    <t>Researched more about the Dart language syntax and using Flutter</t>
+  </si>
+  <si>
+    <t>Check-in: Group meeting with Tyler, discussed what was needed for the pre-alpha build, planning more research for app development</t>
+  </si>
+  <si>
+    <t>Check-in: Group meeting with Tyler, discussed communication between frontend and backend,  tasks to complete, and next steps for group coding session</t>
+  </si>
+  <si>
+    <t>Implemented addPlantView screen, reformatted home screen(route clickable button), and established temporary connection between front/backend. Can get data from the backend server</t>
   </si>
 </sst>
 </file>
@@ -679,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
-  <dimension ref="A1:G199"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,14 +709,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="6">
-        <f>SUM(E4:E199)</f>
-        <v>0.84722222222222243</v>
+        <f>SUM(E4:E200)</f>
+        <v>1.1618055555555558</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -788,7 +797,7 @@
         <v>0.64722222222222225</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" ref="E6:E68" si="0">D6-C6</f>
+        <f t="shared" ref="E6:E69" si="0">D6-C6</f>
         <v>2.2222222222222254E-2</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -854,7 +863,7 @@
         <v>2.2222222222222254E-2</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -875,7 +884,7 @@
         <v>3.4027777777777768E-2</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -883,7 +892,7 @@
         <v>45954</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="9">
         <v>0.62222222222222223</v>
@@ -896,10 +905,10 @@
         <v>0.25972222222222219</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -907,7 +916,7 @@
         <v>45955</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="9">
         <v>0.57291666666666663</v>
@@ -920,41 +929,71 @@
         <v>5.6250000000000022E-2</v>
       </c>
       <c r="F12" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>45964</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.55972222222222223</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>9.8611111111111094E-2</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="15"/>
-    </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="7">
+        <v>45965</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.49305555555555558</v>
+      </c>
       <c r="E14" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="15"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="A15" s="7">
+        <v>45967</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.61527777777777781</v>
+      </c>
       <c r="E15" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="15"/>
+        <f>D15-C15</f>
+        <v>0.19513888888888892</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
@@ -1545,7 +1584,7 @@
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="10">
-        <f t="shared" ref="E69:E132" si="1">D69-C69</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F69" s="15"/>
@@ -1556,7 +1595,7 @@
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E70:E133" si="1">D70-C70</f>
         <v>0</v>
       </c>
       <c r="F70" s="15"/>
@@ -2249,7 +2288,7 @@
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
       <c r="E133" s="10">
-        <f t="shared" ref="E133:E196" si="2">D133-C133</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F133" s="15"/>
@@ -2260,7 +2299,7 @@
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
       <c r="E134" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E134:E197" si="2">D134-C134</f>
         <v>0</v>
       </c>
       <c r="F134" s="15"/>
@@ -2953,7 +2992,7 @@
       <c r="C197" s="8"/>
       <c r="D197" s="8"/>
       <c r="E197" s="10">
-        <f t="shared" ref="E197:E199" si="3">D197-C197</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F197" s="15"/>
@@ -2964,21 +3003,32 @@
       <c r="C198" s="8"/>
       <c r="D198" s="8"/>
       <c r="E198" s="10">
+        <f t="shared" ref="E198:E200" si="3">D198-C198</f>
+        <v>0</v>
+      </c>
+      <c r="F198" s="15"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199" s="11"/>
+      <c r="B199" s="8"/>
+      <c r="C199" s="8"/>
+      <c r="D199" s="8"/>
+      <c r="E199" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F198" s="15"/>
-    </row>
-    <row r="199" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A199" s="12"/>
-      <c r="B199" s="13"/>
-      <c r="C199" s="13"/>
-      <c r="D199" s="13"/>
-      <c r="E199" s="14">
+      <c r="F199" s="15"/>
+    </row>
+    <row r="200" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A200" s="12"/>
+      <c r="B200" s="13"/>
+      <c r="C200" s="13"/>
+      <c r="D200" s="13"/>
+      <c r="E200" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F199" s="16"/>
+      <c r="F200" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated timesheet with research time and start time
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80003F6-FF98-4C6C-B416-CEDC0CC28B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC27FB6-D54D-4240-BB16-5E7C88DE0987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Name:</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Implemented addPlantView screen, reformatted home screen(route clickable button), and established temporary connection between front/backend. Can get data from the backend server</t>
+  </si>
+  <si>
+    <t>Check-in: Group meeting with Tyler, established communicaton between frontend and backend and discussed tasks to complete for the prototype</t>
+  </si>
+  <si>
+    <t>Researching communication from backend to frontend and Flutter mobile app components. GET api call works and can properly pull unformatted data</t>
   </si>
 </sst>
 </file>
@@ -688,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,8 +721,8 @@
         <v>10</v>
       </c>
       <c r="E1" s="6">
-        <f>SUM(E4:E200)</f>
-        <v>1.1618055555555558</v>
+        <f>SUM(E4:E201)</f>
+        <v>0.8090277777777779</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -797,7 +803,7 @@
         <v>0.64722222222222225</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" ref="E6:E69" si="0">D6-C6</f>
+        <f t="shared" ref="E6:E70" si="0">D6-C6</f>
         <v>2.2222222222222254E-2</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -996,35 +1002,61 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="7">
+        <v>45969</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.77222222222222225</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.86458333333333337</v>
+      </c>
       <c r="E16" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="15"/>
+        <f>D16-C16</f>
+        <v>9.2361111111111116E-2</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="7">
+        <v>45971</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.63888888888888884</v>
+      </c>
       <c r="E17" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="15"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="7">
+        <v>45972</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.45902777777777776</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.45902777777777776</v>
       </c>
       <c r="F18" s="15"/>
     </row>
@@ -1595,7 +1627,7 @@
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="10">
-        <f t="shared" ref="E70:E133" si="1">D70-C70</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F70" s="15"/>
@@ -1606,7 +1638,7 @@
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E71:E134" si="1">D71-C71</f>
         <v>0</v>
       </c>
       <c r="F71" s="15"/>
@@ -2299,7 +2331,7 @@
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
       <c r="E134" s="10">
-        <f t="shared" ref="E134:E197" si="2">D134-C134</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F134" s="15"/>
@@ -2310,7 +2342,7 @@
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
       <c r="E135" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E135:E198" si="2">D135-C135</f>
         <v>0</v>
       </c>
       <c r="F135" s="15"/>
@@ -3003,7 +3035,7 @@
       <c r="C198" s="8"/>
       <c r="D198" s="8"/>
       <c r="E198" s="10">
-        <f t="shared" ref="E198:E200" si="3">D198-C198</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F198" s="15"/>
@@ -3014,21 +3046,32 @@
       <c r="C199" s="8"/>
       <c r="D199" s="8"/>
       <c r="E199" s="10">
+        <f t="shared" ref="E199:E201" si="3">D199-C199</f>
+        <v>0</v>
+      </c>
+      <c r="F199" s="15"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" s="11"/>
+      <c r="B200" s="8"/>
+      <c r="C200" s="8"/>
+      <c r="D200" s="8"/>
+      <c r="E200" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F199" s="15"/>
-    </row>
-    <row r="200" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="12"/>
-      <c r="B200" s="13"/>
-      <c r="C200" s="13"/>
-      <c r="D200" s="13"/>
-      <c r="E200" s="14">
+      <c r="F200" s="15"/>
+    </row>
+    <row r="201" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A201" s="12"/>
+      <c r="B201" s="13"/>
+      <c r="C201" s="13"/>
+      <c r="D201" s="13"/>
+      <c r="E201" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F200" s="16"/>
+      <c r="F201" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Base format for post functionality, can fetch plant data from backend, update timesheet
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC27FB6-D54D-4240-BB16-5E7C88DE0987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5774A80-DA4C-4721-A79B-98DE3C7D4299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Name:</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Researching communication from backend to frontend and Flutter mobile app components. GET api call works and can properly pull unformatted data</t>
+  </si>
+  <si>
+    <t>Following tutorials for API calls using http client to communicate with backend. Integrating REST API in Flutter, formatting dart file for posts and displaying in homescreen view</t>
   </si>
 </sst>
 </file>
@@ -696,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +725,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E201)</f>
-        <v>0.8090277777777779</v>
+        <v>1.5458333333333336</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -1053,12 +1056,16 @@
       <c r="C18" s="9">
         <v>0.45902777777777776</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="9">
+        <v>0.7368055555555556</v>
+      </c>
       <c r="E18" s="10">
         <f t="shared" si="0"/>
-        <v>-0.45902777777777776</v>
-      </c>
-      <c r="F18" s="15"/>
+        <v>0.27777777777777785</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>

</xml_diff>

<commit_message>
Updated start/end time, able to display data from backend onto homescreen, currently unformatted
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5774A80-DA4C-4721-A79B-98DE3C7D4299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE65E0D4-9396-4197-BB52-5276605D855B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Name:</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Following tutorials for API calls using http client to communicate with backend. Integrating REST API in Flutter, formatting dart file for posts and displaying in homescreen view</t>
+  </si>
+  <si>
+    <t>Able to properly communicate with the backend and print the data onto the home screen of the mobile application.</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +728,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E201)</f>
-        <v>1.5458333333333336</v>
+        <v>1.7326388888888893</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -1068,15 +1071,25 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="A19" s="7">
+        <v>45974</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.64513888888888893</v>
+      </c>
       <c r="E19" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="15"/>
+        <v>0.18680555555555561</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>

</xml_diff>

<commit_message>
Changed post.dart to plant, changed the format to reflect one plant
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/TimeSheets/TimeReport_SabrinaLuu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE65E0D4-9396-4197-BB52-5276605D855B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB90A81-CEE3-4FFF-AC8E-C8063BF414F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Name:</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Able to properly communicate with the backend and print the data onto the home screen of the mobile application.</t>
+  </si>
+  <si>
+    <t>Reformatting and refactoring homeView, post.dart, and remote_service</t>
   </si>
 </sst>
 </file>
@@ -703,7 +706,7 @@
   <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +731,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E201)</f>
-        <v>1.7326388888888893</v>
+        <v>1.1381944444444447</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -1092,24 +1095,40 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="A20" s="7">
+        <v>45975</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.57986111111111116</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.60277777777777775</v>
+      </c>
       <c r="E20" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="15"/>
+        <v>2.2916666666666585E-2</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="7">
+        <v>45975</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.61736111111111114</v>
+      </c>
       <c r="D21" s="8"/>
       <c r="E21" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.61736111111111114</v>
       </c>
       <c r="F21" s="15"/>
     </row>

</xml_diff>